<commit_message>
2021.06.16 - the rest codes
</commit_message>
<xml_diff>
--- a/10bp.xlsx
+++ b/10bp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="124">
   <si>
     <t>Chr</t>
   </si>
@@ -447,6 +447,14 @@
   </si>
   <si>
     <t>GTTATAAAAA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CACTG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TTTGG</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -820,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -923,19 +931,19 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>68011866</v>
+        <v>1489617</v>
       </c>
       <c r="C5">
-        <v>68012025</v>
+        <v>1489848</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -943,59 +951,59 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>218014792</v>
+        <v>68011866</v>
       </c>
       <c r="C6">
-        <v>218014983</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>68012025</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>45540713</v>
+        <v>218014792</v>
       </c>
       <c r="C7">
-        <v>45540843</v>
-      </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
+        <v>218014983</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>31302612</v>
+        <v>45540713</v>
       </c>
       <c r="C8">
-        <v>31302887</v>
+        <v>45540843</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1003,79 +1011,79 @@
         <v>4</v>
       </c>
       <c r="B9">
+        <v>31302612</v>
+      </c>
+      <c r="C9">
+        <v>31302887</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
         <v>154587696</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>154587891</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>123775491</v>
-      </c>
-      <c r="C10">
-        <v>123775639</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11">
-        <v>150076172</v>
+        <v>123775491</v>
       </c>
       <c r="C11">
-        <v>150076490</v>
+        <v>123775639</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
+        <v>73</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>70277311</v>
+        <v>150076172</v>
       </c>
       <c r="C12">
-        <v>70277444</v>
+        <v>150076490</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1083,39 +1091,39 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <v>91740195</v>
+        <v>70277311</v>
       </c>
       <c r="C13">
-        <v>91740304</v>
+        <v>70277444</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>84160067</v>
+        <v>91740195</v>
       </c>
       <c r="C14">
-        <v>84160301</v>
+        <v>91740304</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>120</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1129,93 +1137,93 @@
         <v>84160301</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>84160067</v>
+      </c>
+      <c r="C16">
+        <v>84160301</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>8</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>124894838</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>124895018</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>77</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>26</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>9</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>77073712</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>77073905</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18">
-        <v>129294197</v>
-      </c>
-      <c r="C18">
-        <v>129294439</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>2170990</v>
+        <v>129294197</v>
       </c>
       <c r="C19">
-        <v>2171176</v>
+        <v>129294439</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1229,10 +1237,10 @@
         <v>2171176</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
         <v>31</v>
@@ -1240,22 +1248,22 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>5983938</v>
+        <v>2170990</v>
       </c>
       <c r="C21">
-        <v>5984088</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>114</v>
+        <v>2171176</v>
+      </c>
+      <c r="D21" t="s">
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1272,7 +1280,7 @@
         <v>114</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
         <v>33</v>
@@ -1292,7 +1300,7 @@
         <v>114</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F23" t="s">
         <v>33</v>
@@ -1303,39 +1311,39 @@
         <v>12</v>
       </c>
       <c r="B24">
-        <v>12296996</v>
+        <v>5983938</v>
       </c>
       <c r="C24">
-        <v>12297220</v>
-      </c>
-      <c r="D24" t="s">
-        <v>79</v>
+        <v>5984088</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25">
-        <v>82147924</v>
+        <v>12296996</v>
       </c>
       <c r="C25">
-        <v>82148108</v>
+        <v>12297220</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="F25" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1352,10 +1360,10 @@
         <v>118</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="F26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1375,52 +1383,51 @@
         <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28">
-        <v>96830983</v>
+        <v>82147924</v>
       </c>
       <c r="C28">
-        <v>96831322</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>81</v>
+        <v>82148108</v>
+      </c>
+      <c r="D28" t="s">
+        <v>118</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>37</v>
+        <v>66</v>
+      </c>
+      <c r="G28" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29">
-        <v>86352651</v>
+        <v>96830983</v>
       </c>
       <c r="C29">
-        <v>86352807</v>
-      </c>
-      <c r="D29" t="s">
-        <v>82</v>
+        <v>96831322</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F29" t="s">
-        <v>39</v>
-      </c>
-      <c r="M29" s="6"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1436,7 +1443,7 @@
         <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="F30" t="s">
         <v>39</v>
@@ -1445,43 +1452,43 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31">
-        <v>74684796</v>
+        <v>86352651</v>
       </c>
       <c r="C31">
-        <v>74684949</v>
+        <v>86352807</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="F31" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="M31" s="6"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32">
-        <v>63281611</v>
+        <v>74684796</v>
       </c>
       <c r="C32">
-        <v>63281916</v>
+        <v>74684949</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="M32" s="6"/>
     </row>
@@ -1502,70 +1509,70 @@
         <v>40</v>
       </c>
       <c r="F33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M33" s="6"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34">
-        <v>29926120</v>
+        <v>63281611</v>
       </c>
       <c r="C34">
-        <v>29926325</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>103</v>
+        <v>63281916</v>
+      </c>
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" t="s">
+        <v>42</v>
       </c>
       <c r="M34" s="6"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35">
-        <v>4525633</v>
+        <v>29926120</v>
       </c>
       <c r="C35">
-        <v>4525789</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>62</v>
+        <v>29926325</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="M35" s="6"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B36">
-        <v>19181941</v>
+        <v>4525633</v>
       </c>
       <c r="C36">
-        <v>19182165</v>
-      </c>
-      <c r="D36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" t="s">
-        <v>44</v>
+        <v>4525789</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="M36" s="6"/>
     </row>
@@ -1574,103 +1581,104 @@
         <v>21</v>
       </c>
       <c r="B37">
-        <v>43636114</v>
+        <v>19181941</v>
       </c>
       <c r="C37">
-        <v>43636543</v>
+        <v>19182165</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M37" s="6"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>43636114</v>
+      </c>
+      <c r="C38">
+        <v>43636543</v>
+      </c>
+      <c r="D38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>22</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>37140258</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>37140413</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>86</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>47</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>121</v>
       </c>
-      <c r="M38" s="6"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39">
-        <v>6869847</v>
-      </c>
-      <c r="C39">
-        <v>6869958</v>
-      </c>
-      <c r="D39" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
       <c r="M39" s="6"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>6869847</v>
+      </c>
+      <c r="C40">
+        <v>6869958</v>
+      </c>
+      <c r="D40" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="M40" s="6"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>11296874</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>11296979</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>87</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E41" s="5"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I44">
-        <v>13</v>
-      </c>
-      <c r="J44">
-        <v>82147924</v>
-      </c>
-      <c r="K44">
-        <v>82148108</v>
-      </c>
-      <c r="L44" t="s">
-        <v>80</v>
-      </c>
-      <c r="M44" t="s">
-        <v>91</v>
-      </c>
-      <c r="N44" t="s">
-        <v>51</v>
-      </c>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E42" s="5"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I45">
@@ -1686,10 +1694,10 @@
         <v>80</v>
       </c>
       <c r="M45" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="N45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -1709,10 +1717,7 @@
         <v>50</v>
       </c>
       <c r="N46" t="s">
-        <v>66</v>
-      </c>
-      <c r="O46" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -1726,22 +1731,16 @@
         <v>82148108</v>
       </c>
       <c r="L47" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="M47" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="N47" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="O47" t="s">
-        <v>93</v>
-      </c>
-      <c r="P47" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -1761,10 +1760,10 @@
         <v>92</v>
       </c>
       <c r="N48" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O48" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P48" t="s">
         <v>94</v>
@@ -1790,27 +1789,56 @@
         <v>92</v>
       </c>
       <c r="N49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O49" t="s">
         <v>97</v>
       </c>
       <c r="P49" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Q49" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="M50" s="5"/>
+      <c r="I50">
+        <v>13</v>
+      </c>
+      <c r="J50">
+        <v>82147924</v>
+      </c>
+      <c r="K50">
+        <v>82148108</v>
+      </c>
+      <c r="L50" t="s">
+        <v>106</v>
+      </c>
+      <c r="M50" t="s">
+        <v>92</v>
+      </c>
+      <c r="N50" t="s">
+        <v>99</v>
+      </c>
+      <c r="O50" t="s">
+        <v>97</v>
+      </c>
+      <c r="P50" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="51" spans="9:17" x14ac:dyDescent="0.25">
       <c r="M51" s="5"/>
     </row>
     <row r="52" spans="9:17" x14ac:dyDescent="0.25">
       <c r="M52" s="5"/>
-      <c r="N52" s="3"/>
+    </row>
+    <row r="53" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="M53" s="5"/>
+      <c r="N53" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>